<commit_message>
Add Referral Hosp Details
</commit_message>
<xml_diff>
--- a/ExcelFiles/ReferralDomain.xlsx
+++ b/ExcelFiles/ReferralDomain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\DemoServerAutomation\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CB3D36-1740-4852-9A6C-18A9FAC10DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE782F6-DE8F-4E19-8864-4FB47E9ACE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,10 +732,10 @@
     <t>vincent</t>
   </si>
   <si>
-    <t>refPat015</t>
-  </si>
-  <si>
-    <t>RefAAH</t>
+    <t>RefAAJ</t>
+  </si>
+  <si>
+    <t>refPat017</t>
   </si>
 </sst>
 </file>
@@ -2357,7 +2357,7 @@
   <dimension ref="A1:AV6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2535,13 +2535,13 @@
     </row>
     <row r="2" spans="1:48" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>108</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>188</v>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="F2" s="6" t="str">
         <f>addPatient!F2</f>
-        <v>RefAAH</v>
+        <v>RefAAJ</v>
       </c>
       <c r="G2" s="6" t="str">
         <f>addPatient!G2</f>
@@ -3038,7 +3038,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
         <f>addPatient!F2</f>
-        <v>RefAAH</v>
+        <v>RefAAJ</v>
       </c>
       <c r="B2" s="6" t="str">
         <f>addPatient!G2</f>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE(A2,".",B2,"@Gmail.com")</f>
-        <v>RefAAH.Riomedtest@Gmail.com</v>
+        <v>RefAAJ.Riomedtest@Gmail.com</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>